<commit_message>
Changed SLR Table to new CFG
</commit_message>
<xml_diff>
--- a/files/SLR Table.xlsx
+++ b/files/SLR Table.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xXcha\Desktop\DHBW\4. Semester\Compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E18F06A-FB34-477D-A2F7-97BE9E051DBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D66181-6741-47DD-9835-74E384C98A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{0BF2FAF1-5BCE-4BFD-94F5-2D50C6FD21E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AQ$82</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="125">
   <si>
     <t>State</t>
   </si>
@@ -113,9 +116,6 @@
     <t>CODE</t>
   </si>
   <si>
-    <t>TYPE</t>
-  </si>
-  <si>
     <t>CODE'</t>
   </si>
   <si>
@@ -174,6 +174,20 @@
   </si>
   <si>
     <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>s</t>
     </r>
     <r>
@@ -182,6 +196,23 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <t>acc</t>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
       <t>2</t>
     </r>
   </si>
@@ -196,7 +227,21 @@
         <color rgb="FF008000"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>1</t>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>4</t>
     </r>
   </si>
   <si>
@@ -209,13 +254,209 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
+      <t>10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>14</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>19</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>23</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>24</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>26</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>27</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
       <t>7</t>
     </r>
   </si>
   <si>
-    <t>acc</t>
-  </si>
-  <si>
     <r>
       <t>r</t>
     </r>
@@ -226,7 +467,7 @@
         <color rgb="FF008000"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>2</t>
+      <t>8</t>
     </r>
   </si>
   <si>
@@ -240,7 +481,7 @@
         <color rgb="FF008000"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>3</t>
+      <t>9</t>
     </r>
   </si>
   <si>
@@ -254,6 +495,607 @@
         <color rgb="FF008000"/>
         <rFont val="Courier"/>
       </rPr>
+      <t>10</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>11</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>12</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>29</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>31</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>20</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>21</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>33</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>26</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>35</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>13</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>16</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>38</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>45</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>28</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>43</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>44</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>23</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>19</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>29</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>52</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>53</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>54</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>55</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>14</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>17</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>27</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>30</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>22</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>62</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>35</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>65</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>66</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>33</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>34</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>72</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>37</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>75</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>32</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>31</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>36</t>
+    </r>
+  </si>
+  <si>
+    <t>LR table</t>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
       <t>4</t>
     </r>
   </si>
@@ -267,7 +1109,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>10</t>
+      <t>5</t>
     </r>
   </si>
   <si>
@@ -280,7 +1122,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>12</t>
+      <t>8</t>
     </r>
   </si>
   <si>
@@ -293,21 +1135,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>9</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>5</t>
+      <t>49</t>
     </r>
   </si>
   <si>
@@ -320,35 +1148,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>14</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>24</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>6</t>
+      <t>51</t>
     </r>
   </si>
   <si>
@@ -361,7 +1161,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>15</t>
+      <t>58</t>
     </r>
   </si>
   <si>
@@ -374,7 +1174,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>25</t>
+      <t>61</t>
     </r>
   </si>
   <si>
@@ -387,7 +1187,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>18</t>
+      <t>64</t>
     </r>
   </si>
   <si>
@@ -400,7 +1200,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>19</t>
+      <t>68</t>
     </r>
   </si>
   <si>
@@ -413,7 +1213,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>20</t>
+      <t>71</t>
     </r>
   </si>
   <si>
@@ -426,7 +1226,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>23</t>
+      <t>74</t>
     </r>
   </si>
   <si>
@@ -439,818 +1239,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>24</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>26</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>27</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>7</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>8</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>9</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>10</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>11</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>12</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>15</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>29</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>18</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>31</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>20</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>21</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>33</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>26</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>35</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>13</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>16</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>38</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>45</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>28</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>43</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>44</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>23</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>46</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>19</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>50</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>29</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>52</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>53</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>54</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>55</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>14</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>17</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>56</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>27</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>30</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>59</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>22</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>62</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>63</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>35</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>65</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>66</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>25</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>38</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>67</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>33</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>69</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>34</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>72</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>73</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>37</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>75</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>32</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>31</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>76</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>78</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>36</t>
+      <t>77</t>
     </r>
   </si>
 </sst>
@@ -1761,16 +1750,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5537F9B5-A9E5-4596-83D2-87E4F1697A55}">
-  <dimension ref="A1:AQ82"/>
+  <dimension ref="A1:AQ81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A1" s="5"/>
+      <c r="A1" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -1811,8 +1802,10 @@
       <c r="AM1" s="6"/>
       <c r="AN1" s="6"/>
       <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="7"/>
+      <c r="AP1" s="7"/>
+      <c r="AQ1" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -1862,8 +1855,8 @@
       <c r="AM2" s="6"/>
       <c r="AN2" s="6"/>
       <c r="AO2" s="6"/>
-      <c r="AP2" s="6"/>
-      <c r="AQ2" s="7"/>
+      <c r="AP2" s="7"/>
+      <c r="AQ2" s="3"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
@@ -1990,18 +1983,18 @@
       <c r="AP3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AQ3" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="AQ3" s="3"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -2025,7 +2018,9 @@
       <c r="X4" s="2">
         <v>1</v>
       </c>
-      <c r="Y4" s="3"/>
+      <c r="Y4" s="2">
+        <v>2</v>
+      </c>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
@@ -2034,7 +2029,9 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
-      <c r="AH4" s="3"/>
+      <c r="AH4" s="2">
+        <v>3</v>
+      </c>
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3"/>
@@ -2050,9 +2047,11 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2072,15 +2071,17 @@
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
       <c r="V5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W5" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X5" s="2">
         <v>1</v>
       </c>
-      <c r="Y5" s="3"/>
+      <c r="Y5" s="2">
+        <v>2</v>
+      </c>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
@@ -2089,7 +2090,9 @@
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
+      <c r="AH5" s="2">
+        <v>3</v>
+      </c>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
@@ -2104,7 +2107,9 @@
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="C6" s="3" t="s">
         <v>47</v>
       </c>
@@ -2126,15 +2131,13 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
+      <c r="V6" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
-      <c r="Y6" s="2">
-        <v>4</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>5</v>
-      </c>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
@@ -2143,9 +2146,7 @@
       <c r="AF6" s="3"/>
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
-      <c r="AI6" s="2">
-        <v>6</v>
-      </c>
+      <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
@@ -2159,8 +2160,12 @@
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -2179,7 +2184,7 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
-      <c r="V7" s="4" t="s">
+      <c r="V7" s="3" t="s">
         <v>48</v>
       </c>
       <c r="W7" s="3"/>
@@ -2208,10 +2213,10 @@
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -2230,9 +2235,7 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
-      <c r="V8" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
@@ -2259,9 +2262,7 @@
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2270,7 +2271,9 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -2281,9 +2284,7 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
-      <c r="V9" s="3" t="s">
-        <v>50</v>
-      </c>
+      <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
@@ -2310,9 +2311,7 @@
       <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -2332,8 +2331,8 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
-      <c r="V10" s="3" t="s">
-        <v>51</v>
+      <c r="V10" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
@@ -2364,19 +2363,17 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="3" t="s">
-        <v>54</v>
-      </c>
+      <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -2391,13 +2388,13 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
+      <c r="Z11" s="2">
+        <v>9</v>
+      </c>
       <c r="AA11" s="2">
-        <v>8</v>
-      </c>
-      <c r="AB11" s="2">
         <v>11</v>
       </c>
+      <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
@@ -2419,42 +2416,30 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="L12" s="3" t="s">
+        <v>87</v>
+      </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="Q12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="V12" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
@@ -2467,7 +2452,9 @@
       <c r="AF12" s="3"/>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
+      <c r="AI12" s="2">
+        <v>13</v>
+      </c>
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
@@ -2482,30 +2469,42 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="L13" s="3"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="O13" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
+      <c r="Q13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
+      <c r="U13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
@@ -2519,9 +2518,7 @@
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
-      <c r="AJ13" s="2">
-        <v>13</v>
-      </c>
+      <c r="AJ13" s="3"/>
       <c r="AK13" s="3"/>
       <c r="AL13" s="3"/>
       <c r="AM13" s="3"/>
@@ -2535,14 +2532,14 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -2554,22 +2551,22 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="V14" s="3" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -2600,7 +2597,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2648,27 +2645,27 @@
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L16" s="3"/>
       <c r="M16" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
@@ -2684,21 +2681,21 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
+      <c r="AB16" s="2">
+        <v>16</v>
+      </c>
       <c r="AC16" s="2">
-        <v>16</v>
-      </c>
-      <c r="AD16" s="2">
         <v>17</v>
       </c>
-      <c r="AE16" s="3"/>
-      <c r="AF16" s="2">
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="2">
         <v>21</v>
       </c>
-      <c r="AG16" s="3"/>
-      <c r="AH16" s="2">
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="2">
         <v>22</v>
       </c>
+      <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
       <c r="AK16" s="3"/>
@@ -2724,7 +2721,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
@@ -2764,7 +2761,7 @@
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -2812,14 +2809,14 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -2831,22 +2828,22 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="V19" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
@@ -2877,7 +2874,7 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -2926,7 +2923,7 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -2975,7 +2972,7 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -3024,7 +3021,7 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -3073,7 +3070,7 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -3122,19 +3119,19 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -3153,10 +3150,10 @@
       <c r="AA25" s="3"/>
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
-      <c r="AD25" s="3"/>
-      <c r="AE25" s="2">
+      <c r="AD25" s="2">
         <v>28</v>
       </c>
+      <c r="AE25" s="3"/>
       <c r="AF25" s="3"/>
       <c r="AG25" s="3"/>
       <c r="AH25" s="3"/>
@@ -3177,21 +3174,21 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
@@ -3212,10 +3209,10 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
-      <c r="AF26" s="3"/>
-      <c r="AG26" s="2">
+      <c r="AF26" s="2">
         <v>30</v>
       </c>
+      <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
       <c r="AI26" s="3"/>
       <c r="AJ26" s="3"/>
@@ -3233,7 +3230,7 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -3243,11 +3240,11 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L27" s="3"/>
       <c r="M27" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
@@ -3264,18 +3261,18 @@
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
-      <c r="AC27" s="3"/>
-      <c r="AD27" s="2">
+      <c r="AC27" s="2">
         <v>32</v>
       </c>
-      <c r="AE27" s="3"/>
-      <c r="AF27" s="2">
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="2">
         <v>21</v>
       </c>
-      <c r="AG27" s="3"/>
-      <c r="AH27" s="2">
+      <c r="AF27" s="3"/>
+      <c r="AG27" s="2">
         <v>22</v>
       </c>
+      <c r="AH27" s="3"/>
       <c r="AI27" s="3"/>
       <c r="AJ27" s="3"/>
       <c r="AK27" s="3"/>
@@ -3293,21 +3290,21 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
@@ -3348,21 +3345,21 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
@@ -3413,7 +3410,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
@@ -3460,13 +3457,13 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
@@ -3487,10 +3484,10 @@
       <c r="AG31" s="3"/>
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
-      <c r="AJ31" s="3"/>
-      <c r="AK31" s="2">
+      <c r="AJ31" s="2">
         <v>34</v>
       </c>
+      <c r="AK31" s="3"/>
       <c r="AL31" s="3"/>
       <c r="AM31" s="3"/>
       <c r="AN31" s="3"/>
@@ -3505,7 +3502,7 @@
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -3515,7 +3512,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
@@ -3555,7 +3552,7 @@
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -3565,11 +3562,11 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L33" s="3"/>
       <c r="M33" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
@@ -3588,14 +3585,14 @@
       <c r="AB33" s="3"/>
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
-      <c r="AE33" s="3"/>
-      <c r="AF33" s="2">
+      <c r="AE33" s="2">
         <v>36</v>
       </c>
-      <c r="AG33" s="3"/>
-      <c r="AH33" s="2">
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="2">
         <v>22</v>
       </c>
+      <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
       <c r="AJ33" s="3"/>
       <c r="AK33" s="3"/>
@@ -3613,19 +3610,19 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
@@ -3665,7 +3662,7 @@
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -3675,11 +3672,11 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L35" s="3"/>
       <c r="M35" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
@@ -3700,10 +3697,10 @@
       <c r="AD35" s="3"/>
       <c r="AE35" s="3"/>
       <c r="AF35" s="3"/>
-      <c r="AG35" s="3"/>
-      <c r="AH35" s="2">
+      <c r="AG35" s="2">
         <v>37</v>
       </c>
+      <c r="AH35" s="3"/>
       <c r="AI35" s="3"/>
       <c r="AJ35" s="3"/>
       <c r="AK35" s="3"/>
@@ -3729,7 +3726,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
@@ -3767,13 +3764,13 @@
       <c r="A37" s="2">
         <v>33</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B37" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
@@ -3785,31 +3782,31 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="P37" s="3"/>
       <c r="Q37" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R37" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
-      <c r="Y37" s="3"/>
-      <c r="Z37" s="2">
+      <c r="Y37" s="2">
         <v>41</v>
       </c>
-      <c r="AA37" s="3"/>
-      <c r="AB37" s="2">
+      <c r="Z37" s="3"/>
+      <c r="AA37" s="2">
         <v>42</v>
       </c>
+      <c r="AB37" s="3"/>
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
       <c r="AE37" s="3"/>
@@ -3818,13 +3815,13 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
       <c r="AJ37" s="3"/>
-      <c r="AK37" s="3"/>
+      <c r="AK37" s="2">
+        <v>39</v>
+      </c>
       <c r="AL37" s="2">
-        <v>39</v>
-      </c>
-      <c r="AM37" s="2">
         <v>40</v>
       </c>
+      <c r="AM37" s="3"/>
       <c r="AN37" s="3"/>
       <c r="AO37" s="3"/>
       <c r="AP37" s="3"/>
@@ -3845,7 +3842,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
@@ -3884,7 +3881,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -3935,19 +3932,19 @@
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -3966,10 +3963,10 @@
       <c r="AA40" s="3"/>
       <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
-      <c r="AD40" s="3"/>
-      <c r="AE40" s="2">
-        <v>47</v>
-      </c>
+      <c r="AD40" s="2">
+        <v>46</v>
+      </c>
+      <c r="AE40" s="3"/>
       <c r="AF40" s="3"/>
       <c r="AG40" s="3"/>
       <c r="AH40" s="3"/>
@@ -3990,21 +3987,21 @@
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -4025,10 +4022,10 @@
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
-      <c r="AF41" s="3"/>
-      <c r="AG41" s="2">
-        <v>48</v>
-      </c>
+      <c r="AF41" s="2">
+        <v>47</v>
+      </c>
+      <c r="AG41" s="3"/>
       <c r="AH41" s="3"/>
       <c r="AI41" s="3"/>
       <c r="AJ41" s="3"/>
@@ -4038,7 +4035,9 @@
       <c r="AN41" s="3"/>
       <c r="AO41" s="3"/>
       <c r="AP41" s="3"/>
-      <c r="AQ41" s="3"/>
+      <c r="AQ41" s="2">
+        <v>49</v>
+      </c>
     </row>
     <row r="42" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
@@ -4047,21 +4046,21 @@
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="K42" s="3"/>
       <c r="L42" s="3" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -4119,7 +4118,7 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
       <c r="U43" s="3" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
@@ -4141,22 +4140,22 @@
       <c r="AM43" s="3"/>
       <c r="AN43" s="3"/>
       <c r="AO43" s="3"/>
-      <c r="AP43" s="3"/>
-      <c r="AQ43" s="2">
-        <v>49</v>
-      </c>
+      <c r="AP43" s="2">
+        <v>48</v>
+      </c>
+      <c r="AQ43" s="3"/>
     </row>
     <row r="44" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>40</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="B44" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -4168,31 +4167,31 @@
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="P44" s="3"/>
       <c r="Q44" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="R44" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
       <c r="U44" s="3" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
-      <c r="Z44" s="2">
+      <c r="Y44" s="2">
         <v>41</v>
       </c>
-      <c r="AA44" s="3"/>
-      <c r="AB44" s="2">
+      <c r="Z44" s="3"/>
+      <c r="AA44" s="2">
         <v>42</v>
       </c>
+      <c r="AB44" s="3"/>
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
       <c r="AE44" s="3"/>
@@ -4201,13 +4200,13 @@
       <c r="AH44" s="3"/>
       <c r="AI44" s="3"/>
       <c r="AJ44" s="3"/>
-      <c r="AK44" s="3"/>
+      <c r="AK44" s="2">
+        <v>50</v>
+      </c>
       <c r="AL44" s="2">
-        <v>51</v>
-      </c>
-      <c r="AM44" s="2">
         <v>40</v>
       </c>
+      <c r="AM44" s="3"/>
       <c r="AN44" s="3"/>
       <c r="AO44" s="3"/>
       <c r="AP44" s="3"/>
@@ -4217,13 +4216,13 @@
       <c r="A45" s="2">
         <v>41</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3" t="s">
-        <v>94</v>
-      </c>
+      <c r="B45" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -4235,19 +4234,19 @@
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="P45" s="3"/>
       <c r="Q45" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="R45" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
       <c r="U45" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
@@ -4279,7 +4278,7 @@
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -4335,7 +4334,7 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
@@ -4384,7 +4383,7 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
@@ -4424,13 +4423,11 @@
         <v>45</v>
       </c>
       <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="C49" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -4452,12 +4449,8 @@
       <c r="X49" s="3"/>
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
-      <c r="AA49" s="2">
-        <v>8</v>
-      </c>
-      <c r="AB49" s="2">
-        <v>11</v>
-      </c>
+      <c r="AA49" s="3"/>
+      <c r="AB49" s="3"/>
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
       <c r="AE49" s="3"/>
@@ -4479,10 +4472,10 @@
         <v>46</v>
       </c>
       <c r="B50" s="3"/>
-      <c r="C50" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -4490,7 +4483,9 @@
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
+      <c r="L50" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
@@ -4530,17 +4525,19 @@
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
+      <c r="I51" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -4580,24 +4577,20 @@
       </c>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
-      <c r="D52" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
-      <c r="L52" s="3" t="s">
-        <v>100</v>
-      </c>
+      <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
+      <c r="O52" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
@@ -4632,21 +4625,31 @@
         <v>49</v>
       </c>
       <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
+      <c r="C53" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
+      <c r="F53" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
+      <c r="K53" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
+      <c r="M53" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="N53" s="3"/>
-      <c r="O53" s="3" t="s">
-        <v>101</v>
-      </c>
+      <c r="O53" s="3"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3"/>
       <c r="R53" s="3"/>
@@ -4659,12 +4662,20 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
       <c r="AA53" s="3"/>
-      <c r="AB53" s="3"/>
-      <c r="AC53" s="3"/>
+      <c r="AB53" s="2">
+        <v>56</v>
+      </c>
+      <c r="AC53" s="2">
+        <v>17</v>
+      </c>
       <c r="AD53" s="3"/>
-      <c r="AE53" s="3"/>
+      <c r="AE53" s="2">
+        <v>21</v>
+      </c>
       <c r="AF53" s="3"/>
-      <c r="AG53" s="3"/>
+      <c r="AG53" s="2">
+        <v>22</v>
+      </c>
       <c r="AH53" s="3"/>
       <c r="AI53" s="3"/>
       <c r="AJ53" s="3"/>
@@ -4681,37 +4692,29 @@
         <v>50</v>
       </c>
       <c r="B54" s="3"/>
-      <c r="C54" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
-      <c r="K54" s="3" t="s">
-        <v>64</v>
-      </c>
+      <c r="K54" s="3"/>
       <c r="L54" s="3"/>
-      <c r="M54" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="M54" s="3"/>
       <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
+      <c r="O54" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
       <c r="R54" s="3"/>
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
-      <c r="U54" s="3"/>
+      <c r="U54" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="V54" s="3"/>
       <c r="W54" s="3"/>
       <c r="X54" s="3"/>
@@ -4719,20 +4722,12 @@
       <c r="Z54" s="3"/>
       <c r="AA54" s="3"/>
       <c r="AB54" s="3"/>
-      <c r="AC54" s="2">
-        <v>57</v>
-      </c>
-      <c r="AD54" s="2">
-        <v>17</v>
-      </c>
+      <c r="AC54" s="3"/>
+      <c r="AD54" s="3"/>
       <c r="AE54" s="3"/>
-      <c r="AF54" s="2">
-        <v>21</v>
-      </c>
+      <c r="AF54" s="3"/>
       <c r="AG54" s="3"/>
-      <c r="AH54" s="2">
-        <v>22</v>
-      </c>
+      <c r="AH54" s="3"/>
       <c r="AI54" s="3"/>
       <c r="AJ54" s="3"/>
       <c r="AK54" s="3"/>
@@ -4747,10 +4742,14 @@
       <c r="A55" s="2">
         <v>51</v>
       </c>
-      <c r="B55" s="3"/>
+      <c r="B55" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
@@ -4761,15 +4760,19 @@
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
       <c r="O55" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
+      <c r="Q55" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="R55" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="S55" s="3"/>
       <c r="T55" s="3"/>
       <c r="U55" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="V55" s="3"/>
       <c r="W55" s="3"/>
@@ -4799,37 +4802,27 @@
         <v>52</v>
       </c>
       <c r="B56" s="3"/>
-      <c r="C56" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="C56" s="3"/>
       <c r="D56" s="3"/>
-      <c r="E56" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
+      <c r="H56" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
-      <c r="O56" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="O56" s="3"/>
       <c r="P56" s="3"/>
-      <c r="Q56" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="R56" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
       <c r="S56" s="3"/>
       <c r="T56" s="3"/>
-      <c r="U56" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="U56" s="3"/>
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
@@ -4847,7 +4840,9 @@
       <c r="AJ56" s="3"/>
       <c r="AK56" s="3"/>
       <c r="AL56" s="3"/>
-      <c r="AM56" s="3"/>
+      <c r="AM56" s="2">
+        <v>57</v>
+      </c>
       <c r="AN56" s="3"/>
       <c r="AO56" s="3"/>
       <c r="AP56" s="3"/>
@@ -4864,7 +4859,7 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
@@ -4896,10 +4891,10 @@
       <c r="AJ57" s="3"/>
       <c r="AK57" s="3"/>
       <c r="AL57" s="3"/>
-      <c r="AM57" s="3"/>
-      <c r="AN57" s="2">
-        <v>58</v>
-      </c>
+      <c r="AM57" s="2">
+        <v>59</v>
+      </c>
+      <c r="AN57" s="3"/>
       <c r="AO57" s="3"/>
       <c r="AP57" s="3"/>
       <c r="AQ57" s="3"/>
@@ -4914,17 +4909,19 @@
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
-      <c r="H58" s="3" t="s">
-        <v>104</v>
-      </c>
+      <c r="H58" s="3"/>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
+      <c r="L58" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
+      <c r="P58" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
       <c r="S58" s="3"/>
@@ -4944,13 +4941,13 @@
       <c r="AG58" s="3"/>
       <c r="AH58" s="3"/>
       <c r="AI58" s="3"/>
-      <c r="AJ58" s="3"/>
+      <c r="AJ58" s="2">
+        <v>60</v>
+      </c>
       <c r="AK58" s="3"/>
       <c r="AL58" s="3"/>
       <c r="AM58" s="3"/>
-      <c r="AN58" s="2">
-        <v>60</v>
-      </c>
+      <c r="AN58" s="3"/>
       <c r="AO58" s="3"/>
       <c r="AP58" s="3"/>
       <c r="AQ58" s="3"/>
@@ -4959,8 +4956,12 @@
       <c r="A59" s="2">
         <v>55</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
+      <c r="B59" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
@@ -4969,21 +4970,19 @@
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
-      <c r="L59" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
-      <c r="P59" s="3" t="s">
-        <v>82</v>
-      </c>
+      <c r="P59" s="3"/>
       <c r="Q59" s="3"/>
       <c r="R59" s="3"/>
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
       <c r="U59" s="3"/>
-      <c r="V59" s="3"/>
+      <c r="V59" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
       <c r="Y59" s="3"/>
@@ -4998,9 +4997,7 @@
       <c r="AH59" s="3"/>
       <c r="AI59" s="3"/>
       <c r="AJ59" s="3"/>
-      <c r="AK59" s="2">
-        <v>61</v>
-      </c>
+      <c r="AK59" s="3"/>
       <c r="AL59" s="3"/>
       <c r="AM59" s="3"/>
       <c r="AN59" s="3"/>
@@ -5012,11 +5009,11 @@
       <c r="A60" s="2">
         <v>56</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="B60" s="3"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="D60" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -5034,9 +5031,7 @@
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
-      <c r="V60" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="V60" s="3"/>
       <c r="W60" s="3"/>
       <c r="X60" s="3"/>
       <c r="Y60" s="3"/>
@@ -5065,9 +5060,7 @@
       </c>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
-      <c r="D61" s="3" t="s">
-        <v>106</v>
-      </c>
+      <c r="D61" s="3"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -5075,7 +5068,9 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
+      <c r="L61" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
@@ -5123,7 +5118,7 @@
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M62" s="3"/>
       <c r="N62" s="3"/>
@@ -5131,7 +5126,9 @@
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
       <c r="R62" s="3"/>
-      <c r="S62" s="3"/>
+      <c r="S62" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
       <c r="V62" s="3"/>
@@ -5152,7 +5149,9 @@
       <c r="AK62" s="3"/>
       <c r="AL62" s="3"/>
       <c r="AM62" s="3"/>
-      <c r="AN62" s="3"/>
+      <c r="AN62" s="2">
+        <v>63</v>
+      </c>
       <c r="AO62" s="3"/>
       <c r="AP62" s="3"/>
       <c r="AQ62" s="3"/>
@@ -5172,7 +5171,7 @@
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
@@ -5180,9 +5179,7 @@
       <c r="P63" s="3"/>
       <c r="Q63" s="3"/>
       <c r="R63" s="3"/>
-      <c r="S63" s="3" t="s">
-        <v>109</v>
-      </c>
+      <c r="S63" s="3"/>
       <c r="T63" s="3"/>
       <c r="U63" s="3"/>
       <c r="V63" s="3"/>
@@ -5204,9 +5201,7 @@
       <c r="AL63" s="3"/>
       <c r="AM63" s="3"/>
       <c r="AN63" s="3"/>
-      <c r="AO63" s="2">
-        <v>64</v>
-      </c>
+      <c r="AO63" s="3"/>
       <c r="AP63" s="3"/>
       <c r="AQ63" s="3"/>
     </row>
@@ -5225,7 +5220,7 @@
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3" t="s">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
@@ -5273,12 +5268,12 @@
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
-      <c r="L65" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="L65" s="3"/>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
-      <c r="O65" s="3"/>
+      <c r="O65" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="P65" s="3"/>
       <c r="Q65" s="3"/>
       <c r="R65" s="3"/>
@@ -5324,10 +5319,10 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
-      <c r="O66" s="3" t="s">
-        <v>112</v>
-      </c>
+      <c r="N66" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="O66" s="3"/>
       <c r="P66" s="3"/>
       <c r="Q66" s="3"/>
       <c r="R66" s="3"/>
@@ -5371,11 +5366,11 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
+      <c r="L67" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="M67" s="3"/>
-      <c r="N67" s="3" t="s">
-        <v>113</v>
-      </c>
+      <c r="N67" s="3"/>
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
@@ -5416,13 +5411,13 @@
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
+      <c r="H68" s="3" t="s">
+        <v>118</v>
+      </c>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
-      <c r="L68" s="3" t="s">
-        <v>114</v>
-      </c>
+      <c r="L68" s="3"/>
       <c r="M68" s="3"/>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
@@ -5449,7 +5444,9 @@
       <c r="AJ68" s="3"/>
       <c r="AK68" s="3"/>
       <c r="AL68" s="3"/>
-      <c r="AM68" s="3"/>
+      <c r="AM68" s="2">
+        <v>67</v>
+      </c>
       <c r="AN68" s="3"/>
       <c r="AO68" s="3"/>
       <c r="AP68" s="3"/>
@@ -5465,15 +5462,15 @@
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
-      <c r="H69" s="3" t="s">
-        <v>104</v>
-      </c>
+      <c r="H69" s="3"/>
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
       <c r="M69" s="3"/>
-      <c r="N69" s="3"/>
+      <c r="N69" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
       <c r="Q69" s="3"/>
@@ -5499,9 +5496,7 @@
       <c r="AK69" s="3"/>
       <c r="AL69" s="3"/>
       <c r="AM69" s="3"/>
-      <c r="AN69" s="2">
-        <v>68</v>
-      </c>
+      <c r="AN69" s="3"/>
       <c r="AO69" s="3"/>
       <c r="AP69" s="3"/>
       <c r="AQ69" s="3"/>
@@ -5510,10 +5505,14 @@
       <c r="A70" s="2">
         <v>66</v>
       </c>
-      <c r="B70" s="3"/>
+      <c r="B70" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
+      <c r="E70" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
@@ -5522,22 +5521,32 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
-      <c r="N70" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="O70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="P70" s="3"/>
-      <c r="Q70" s="3"/>
-      <c r="R70" s="3"/>
+      <c r="Q70" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R70" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
-      <c r="U70" s="3"/>
+      <c r="U70" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="V70" s="3"/>
       <c r="W70" s="3"/>
       <c r="X70" s="3"/>
-      <c r="Y70" s="3"/>
+      <c r="Y70" s="2">
+        <v>41</v>
+      </c>
       <c r="Z70" s="3"/>
-      <c r="AA70" s="3"/>
+      <c r="AA70" s="2">
+        <v>42</v>
+      </c>
       <c r="AB70" s="3"/>
       <c r="AC70" s="3"/>
       <c r="AD70" s="3"/>
@@ -5547,8 +5556,12 @@
       <c r="AH70" s="3"/>
       <c r="AI70" s="3"/>
       <c r="AJ70" s="3"/>
-      <c r="AK70" s="3"/>
-      <c r="AL70" s="3"/>
+      <c r="AK70" s="2">
+        <v>69</v>
+      </c>
+      <c r="AL70" s="2">
+        <v>40</v>
+      </c>
       <c r="AM70" s="3"/>
       <c r="AN70" s="3"/>
       <c r="AO70" s="3"/>
@@ -5560,48 +5573,34 @@
         <v>67</v>
       </c>
       <c r="B71" s="3"/>
-      <c r="C71" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="C71" s="3"/>
       <c r="D71" s="3"/>
-      <c r="E71" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
+      <c r="L71" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="M71" s="3"/>
       <c r="N71" s="3"/>
-      <c r="O71" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="O71" s="3"/>
       <c r="P71" s="3"/>
-      <c r="Q71" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="R71" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
       <c r="S71" s="3"/>
       <c r="T71" s="3"/>
-      <c r="U71" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="U71" s="3"/>
       <c r="V71" s="3"/>
       <c r="W71" s="3"/>
       <c r="X71" s="3"/>
       <c r="Y71" s="3"/>
-      <c r="Z71" s="2">
-        <v>41</v>
-      </c>
+      <c r="Z71" s="3"/>
       <c r="AA71" s="3"/>
-      <c r="AB71" s="2">
-        <v>42</v>
-      </c>
+      <c r="AB71" s="3"/>
       <c r="AC71" s="3"/>
       <c r="AD71" s="3"/>
       <c r="AE71" s="3"/>
@@ -5611,12 +5610,8 @@
       <c r="AI71" s="3"/>
       <c r="AJ71" s="3"/>
       <c r="AK71" s="3"/>
-      <c r="AL71" s="2">
-        <v>70</v>
-      </c>
-      <c r="AM71" s="2">
-        <v>40</v>
-      </c>
+      <c r="AL71" s="3"/>
+      <c r="AM71" s="3"/>
       <c r="AN71" s="3"/>
       <c r="AO71" s="3"/>
       <c r="AP71" s="3"/>
@@ -5626,34 +5621,48 @@
       <c r="A72" s="2">
         <v>68</v>
       </c>
-      <c r="B72" s="3"/>
+      <c r="B72" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
+      <c r="E72" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
-      <c r="L72" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="L72" s="3"/>
       <c r="M72" s="3"/>
       <c r="N72" s="3"/>
-      <c r="O72" s="3"/>
+      <c r="O72" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="P72" s="3"/>
-      <c r="Q72" s="3"/>
-      <c r="R72" s="3"/>
+      <c r="Q72" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R72" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="S72" s="3"/>
       <c r="T72" s="3"/>
-      <c r="U72" s="3"/>
+      <c r="U72" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="V72" s="3"/>
       <c r="W72" s="3"/>
       <c r="X72" s="3"/>
-      <c r="Y72" s="3"/>
+      <c r="Y72" s="2">
+        <v>41</v>
+      </c>
       <c r="Z72" s="3"/>
-      <c r="AA72" s="3"/>
+      <c r="AA72" s="2">
+        <v>42</v>
+      </c>
       <c r="AB72" s="3"/>
       <c r="AC72" s="3"/>
       <c r="AD72" s="3"/>
@@ -5663,8 +5672,12 @@
       <c r="AH72" s="3"/>
       <c r="AI72" s="3"/>
       <c r="AJ72" s="3"/>
-      <c r="AK72" s="3"/>
-      <c r="AL72" s="3"/>
+      <c r="AK72" s="2">
+        <v>70</v>
+      </c>
+      <c r="AL72" s="2">
+        <v>40</v>
+      </c>
       <c r="AM72" s="3"/>
       <c r="AN72" s="3"/>
       <c r="AO72" s="3"/>
@@ -5676,13 +5689,9 @@
         <v>69</v>
       </c>
       <c r="B73" s="3"/>
-      <c r="C73" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="C73" s="3"/>
       <c r="D73" s="3"/>
-      <c r="E73" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
@@ -5693,31 +5702,21 @@
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
       <c r="O73" s="3" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="P73" s="3"/>
-      <c r="Q73" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="R73" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
       <c r="S73" s="3"/>
       <c r="T73" s="3"/>
-      <c r="U73" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="U73" s="3"/>
       <c r="V73" s="3"/>
       <c r="W73" s="3"/>
       <c r="X73" s="3"/>
       <c r="Y73" s="3"/>
-      <c r="Z73" s="2">
-        <v>41</v>
-      </c>
+      <c r="Z73" s="3"/>
       <c r="AA73" s="3"/>
-      <c r="AB73" s="2">
-        <v>42</v>
-      </c>
+      <c r="AB73" s="3"/>
       <c r="AC73" s="3"/>
       <c r="AD73" s="3"/>
       <c r="AE73" s="3"/>
@@ -5727,12 +5726,8 @@
       <c r="AI73" s="3"/>
       <c r="AJ73" s="3"/>
       <c r="AK73" s="3"/>
-      <c r="AL73" s="2">
-        <v>71</v>
-      </c>
-      <c r="AM73" s="2">
-        <v>40</v>
-      </c>
+      <c r="AL73" s="3"/>
+      <c r="AM73" s="3"/>
       <c r="AN73" s="3"/>
       <c r="AO73" s="3"/>
       <c r="AP73" s="3"/>
@@ -5756,7 +5751,7 @@
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
       <c r="O74" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="P74" s="3"/>
       <c r="Q74" s="3"/>
@@ -5791,10 +5786,14 @@
       <c r="A75" s="2">
         <v>71</v>
       </c>
-      <c r="B75" s="3"/>
+      <c r="B75" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
+      <c r="E75" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
@@ -5805,14 +5804,22 @@
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
       <c r="O75" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="P75" s="3"/>
-      <c r="Q75" s="3"/>
-      <c r="R75" s="3"/>
+      <c r="Q75" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="R75" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="S75" s="3"/>
-      <c r="T75" s="3"/>
-      <c r="U75" s="3"/>
+      <c r="T75" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="U75" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="V75" s="3"/>
       <c r="W75" s="3"/>
       <c r="X75" s="3"/>
@@ -5832,7 +5839,9 @@
       <c r="AL75" s="3"/>
       <c r="AM75" s="3"/>
       <c r="AN75" s="3"/>
-      <c r="AO75" s="3"/>
+      <c r="AO75" s="2">
+        <v>73</v>
+      </c>
       <c r="AP75" s="3"/>
       <c r="AQ75" s="3"/>
     </row>
@@ -5840,13 +5849,13 @@
       <c r="A76" s="2">
         <v>72</v>
       </c>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3" t="s">
-        <v>119</v>
-      </c>
+      <c r="B76" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C76" s="3"/>
       <c r="D76" s="3"/>
       <c r="E76" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
@@ -5858,21 +5867,19 @@
       <c r="M76" s="3"/>
       <c r="N76" s="3"/>
       <c r="O76" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="P76" s="3"/>
       <c r="Q76" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="R76" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="S76" s="3"/>
-      <c r="T76" s="3" t="s">
-        <v>120</v>
-      </c>
+      <c r="T76" s="3"/>
       <c r="U76" s="3" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="V76" s="3"/>
       <c r="W76" s="3"/>
@@ -5894,22 +5901,20 @@
       <c r="AM76" s="3"/>
       <c r="AN76" s="3"/>
       <c r="AO76" s="3"/>
-      <c r="AP76" s="2">
-        <v>74</v>
-      </c>
+      <c r="AP76" s="3"/>
       <c r="AQ76" s="3"/>
     </row>
     <row r="77" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>73</v>
       </c>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3" t="s">
-        <v>121</v>
-      </c>
+      <c r="B77" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -5921,19 +5926,19 @@
       <c r="M77" s="3"/>
       <c r="N77" s="3"/>
       <c r="O77" s="3" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="P77" s="3"/>
       <c r="Q77" s="3" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="R77" s="3" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="S77" s="3"/>
       <c r="T77" s="3"/>
       <c r="U77" s="3" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
       <c r="V77" s="3"/>
       <c r="W77" s="3"/>
@@ -5963,13 +5968,9 @@
         <v>74</v>
       </c>
       <c r="B78" s="3"/>
-      <c r="C78" s="3" t="s">
-        <v>122</v>
-      </c>
+      <c r="C78" s="3"/>
       <c r="D78" s="3"/>
-      <c r="E78" s="3" t="s">
-        <v>122</v>
-      </c>
+      <c r="E78" s="3"/>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
@@ -5978,22 +5979,16 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
       <c r="M78" s="3"/>
-      <c r="N78" s="3"/>
-      <c r="O78" s="3" t="s">
-        <v>122</v>
-      </c>
+      <c r="N78" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="O78" s="3"/>
       <c r="P78" s="3"/>
-      <c r="Q78" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="R78" s="3" t="s">
-        <v>122</v>
-      </c>
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
       <c r="S78" s="3"/>
       <c r="T78" s="3"/>
-      <c r="U78" s="3" t="s">
-        <v>122</v>
-      </c>
+      <c r="U78" s="3"/>
       <c r="V78" s="3"/>
       <c r="W78" s="3"/>
       <c r="X78" s="3"/>
@@ -6021,10 +6016,14 @@
       <c r="A79" s="2">
         <v>75</v>
       </c>
-      <c r="B79" s="3"/>
+      <c r="B79" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
+      <c r="E79" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
@@ -6033,22 +6032,32 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
       <c r="M79" s="3"/>
-      <c r="N79" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="O79" s="3"/>
+      <c r="N79" s="3"/>
+      <c r="O79" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="P79" s="3"/>
-      <c r="Q79" s="3"/>
-      <c r="R79" s="3"/>
+      <c r="Q79" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R79" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="S79" s="3"/>
       <c r="T79" s="3"/>
-      <c r="U79" s="3"/>
+      <c r="U79" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="V79" s="3"/>
       <c r="W79" s="3"/>
       <c r="X79" s="3"/>
-      <c r="Y79" s="3"/>
+      <c r="Y79" s="2">
+        <v>41</v>
+      </c>
       <c r="Z79" s="3"/>
-      <c r="AA79" s="3"/>
+      <c r="AA79" s="2">
+        <v>42</v>
+      </c>
       <c r="AB79" s="3"/>
       <c r="AC79" s="3"/>
       <c r="AD79" s="3"/>
@@ -6058,8 +6067,12 @@
       <c r="AH79" s="3"/>
       <c r="AI79" s="3"/>
       <c r="AJ79" s="3"/>
-      <c r="AK79" s="3"/>
-      <c r="AL79" s="3"/>
+      <c r="AK79" s="2">
+        <v>76</v>
+      </c>
+      <c r="AL79" s="2">
+        <v>40</v>
+      </c>
       <c r="AM79" s="3"/>
       <c r="AN79" s="3"/>
       <c r="AO79" s="3"/>
@@ -6071,13 +6084,9 @@
         <v>76</v>
       </c>
       <c r="B80" s="3"/>
-      <c r="C80" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="C80" s="3"/>
       <c r="D80" s="3"/>
-      <c r="E80" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="E80" s="3"/>
       <c r="F80" s="3"/>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
@@ -6088,31 +6097,21 @@
       <c r="M80" s="3"/>
       <c r="N80" s="3"/>
       <c r="O80" s="3" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
       <c r="P80" s="3"/>
-      <c r="Q80" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="R80" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
       <c r="S80" s="3"/>
       <c r="T80" s="3"/>
-      <c r="U80" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="U80" s="3"/>
       <c r="V80" s="3"/>
       <c r="W80" s="3"/>
       <c r="X80" s="3"/>
       <c r="Y80" s="3"/>
-      <c r="Z80" s="2">
-        <v>41</v>
-      </c>
+      <c r="Z80" s="3"/>
       <c r="AA80" s="3"/>
-      <c r="AB80" s="2">
-        <v>42</v>
-      </c>
+      <c r="AB80" s="3"/>
       <c r="AC80" s="3"/>
       <c r="AD80" s="3"/>
       <c r="AE80" s="3"/>
@@ -6122,25 +6121,25 @@
       <c r="AI80" s="3"/>
       <c r="AJ80" s="3"/>
       <c r="AK80" s="3"/>
-      <c r="AL80" s="2">
-        <v>77</v>
-      </c>
-      <c r="AM80" s="2">
-        <v>40</v>
-      </c>
+      <c r="AL80" s="3"/>
+      <c r="AM80" s="3"/>
       <c r="AN80" s="3"/>
       <c r="AO80" s="3"/>
       <c r="AP80" s="3"/>
       <c r="AQ80" s="3"/>
     </row>
-    <row r="81" spans="1:43" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>77</v>
       </c>
-      <c r="B81" s="3"/>
+      <c r="B81" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
+      <c r="E81" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
@@ -6151,14 +6150,20 @@
       <c r="M81" s="3"/>
       <c r="N81" s="3"/>
       <c r="O81" s="3" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="P81" s="3"/>
-      <c r="Q81" s="3"/>
-      <c r="R81" s="3"/>
+      <c r="Q81" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="R81" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
-      <c r="U81" s="3"/>
+      <c r="U81" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="V81" s="3"/>
       <c r="W81" s="3"/>
       <c r="X81" s="3"/>
@@ -6180,74 +6185,15 @@
       <c r="AN81" s="3"/>
       <c r="AO81" s="3"/>
       <c r="AP81" s="3"/>
-      <c r="AQ81" s="3"/>
-    </row>
-    <row r="82" spans="1:43" x14ac:dyDescent="0.35">
-      <c r="A82" s="2">
-        <v>78</v>
-      </c>
-      <c r="B82" s="3"/>
-      <c r="C82" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
-      <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
-      <c r="M82" s="3"/>
-      <c r="N82" s="3"/>
-      <c r="O82" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="P82" s="3"/>
-      <c r="Q82" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="R82" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="S82" s="3"/>
-      <c r="T82" s="3"/>
-      <c r="U82" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="V82" s="3"/>
-      <c r="W82" s="3"/>
-      <c r="X82" s="3"/>
-      <c r="Y82" s="3"/>
-      <c r="Z82" s="3"/>
-      <c r="AA82" s="3"/>
-      <c r="AB82" s="3"/>
-      <c r="AC82" s="3"/>
-      <c r="AD82" s="3"/>
-      <c r="AE82" s="3"/>
-      <c r="AF82" s="3"/>
-      <c r="AG82" s="3"/>
-      <c r="AH82" s="3"/>
-      <c r="AI82" s="3"/>
-      <c r="AJ82" s="3"/>
-      <c r="AK82" s="3"/>
-      <c r="AL82" s="3"/>
-      <c r="AM82" s="3"/>
-      <c r="AN82" s="3"/>
-      <c r="AO82" s="3"/>
-      <c r="AP82" s="3"/>
-      <c r="AQ82" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:AQ1"/>
+    <mergeCell ref="A1:AP1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:V2"/>
-    <mergeCell ref="W2:AQ2"/>
+    <mergeCell ref="W2:AP2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed SLR table for CFG
</commit_message>
<xml_diff>
--- a/files/SLR Table.xlsx
+++ b/files/SLR Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xXcha\Desktop\DHBW\4. Semester\Compiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xXcha\CompilerTermProject\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D66181-6741-47DD-9835-74E384C98A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652CD140-F2D8-40B5-B20B-A6C291514313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{0BF2FAF1-5BCE-4BFD-94F5-2D50C6FD21E6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="128">
   <si>
     <t>State</t>
   </si>
@@ -908,6 +908,20 @@
   </si>
   <si>
     <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>35</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>s</t>
     </r>
     <r>
@@ -916,7 +930,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>62</t>
+      <t>66</t>
     </r>
   </si>
   <si>
@@ -930,8 +944,95 @@
         <color rgb="FF008000"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>35</t>
-    </r>
+      <t>25</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>33</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>34</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>37</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>32</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>31</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>36</t>
+    </r>
+  </si>
+  <si>
+    <t>LR table</t>
   </si>
   <si>
     <r>
@@ -943,7 +1044,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>65</t>
+      <t>49</t>
     </r>
   </si>
   <si>
@@ -956,7 +1057,153 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>66</t>
+      <t>64</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>68</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>74</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>77</t>
+    </r>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>41</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>56</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>57</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>60</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>63</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Courier"/>
+      </rPr>
+      <t>67</t>
     </r>
   </si>
   <si>
@@ -970,35 +1217,7 @@
         <color rgb="FF008000"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>25</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>33</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>34</t>
+      <t>38</t>
     </r>
   </si>
   <si>
@@ -1011,21 +1230,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>72</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>37</t>
+      <t>70</t>
     </r>
   </si>
   <si>
@@ -1038,53 +1243,8 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>75</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>32</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>31</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>r</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF008000"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>36</t>
-    </r>
-  </si>
-  <si>
-    <t>LR table</t>
+      <t>73</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1096,7 +1256,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>4</t>
+      <t>76</t>
     </r>
   </si>
   <si>
@@ -1109,137 +1269,7 @@
         <color rgb="FF0000FF"/>
         <rFont val="Courier"/>
       </rPr>
-      <t>5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>8</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>49</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>51</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>58</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>61</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>64</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>68</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>71</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>74</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Courier"/>
-      </rPr>
-      <t>77</t>
+      <t>79</t>
     </r>
   </si>
 </sst>
@@ -1750,17 +1780,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5537F9B5-A9E5-4596-83D2-87E4F1697A55}">
-  <dimension ref="A1:AQ81"/>
+  <dimension ref="A1:AQ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="73" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1802,10 +1832,8 @@
       <c r="AM1" s="6"/>
       <c r="AN1" s="6"/>
       <c r="AO1" s="6"/>
-      <c r="AP1" s="7"/>
-      <c r="AQ1" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="AP1" s="6"/>
+      <c r="AQ1" s="7"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -1855,8 +1883,8 @@
       <c r="AM2" s="6"/>
       <c r="AN2" s="6"/>
       <c r="AO2" s="6"/>
-      <c r="AP2" s="7"/>
-      <c r="AQ2" s="3"/>
+      <c r="AP2" s="6"/>
+      <c r="AQ2" s="7"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
@@ -1927,74 +1955,74 @@
         <v>24</v>
       </c>
       <c r="X3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AJ3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AJ3" s="1" t="s">
+      <c r="AK3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AL3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AM3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AN3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AN3" s="1" t="s">
+      <c r="AO3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AO3" s="1" t="s">
+      <c r="AP3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AP3" s="1" t="s">
+      <c r="AQ3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AQ3" s="3"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>114</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -2018,9 +2046,7 @@
       <c r="X4" s="2">
         <v>1</v>
       </c>
-      <c r="Y4" s="2">
-        <v>2</v>
-      </c>
+      <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
@@ -2029,9 +2055,7 @@
       <c r="AE4" s="3"/>
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
-      <c r="AH4" s="2">
-        <v>3</v>
-      </c>
+      <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3"/>
@@ -2047,11 +2071,9 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>114</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -2074,14 +2096,12 @@
         <v>44</v>
       </c>
       <c r="W5" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X5" s="2">
         <v>1</v>
       </c>
-      <c r="Y5" s="2">
-        <v>2</v>
-      </c>
+      <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
@@ -2090,9 +2110,7 @@
       <c r="AE5" s="3"/>
       <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
-      <c r="AH5" s="2">
-        <v>3</v>
-      </c>
+      <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
@@ -2107,11 +2125,9 @@
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -2131,13 +2147,15 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
-      <c r="V6" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
+      <c r="Y6" s="2">
+        <v>4</v>
+      </c>
+      <c r="Z6" s="2">
+        <v>5</v>
+      </c>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
@@ -2146,7 +2164,9 @@
       <c r="AF6" s="3"/>
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
+      <c r="AI6" s="2">
+        <v>6</v>
+      </c>
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
       <c r="AL6" s="3"/>
@@ -2160,12 +2180,8 @@
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>48</v>
-      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -2184,8 +2200,8 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
-      <c r="V7" s="3" t="s">
-        <v>48</v>
+      <c r="V7" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
@@ -2213,10 +2229,10 @@
       <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>45</v>
-      </c>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -2235,7 +2251,9 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
+      <c r="V8" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
@@ -2262,7 +2280,9 @@
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -2271,9 +2291,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="3" t="s">
-        <v>115</v>
-      </c>
+      <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
@@ -2284,7 +2302,9 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
+      <c r="V9" s="3" t="s">
+        <v>48</v>
+      </c>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
@@ -2311,7 +2331,9 @@
       <c r="A10" s="2">
         <v>6</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -2331,8 +2353,8 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
-      <c r="V10" s="4" t="s">
-        <v>46</v>
+      <c r="V10" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
@@ -2373,7 +2395,9 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="K11" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -2388,13 +2412,13 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
-      <c r="Z11" s="2">
-        <v>9</v>
-      </c>
+      <c r="Z11" s="3"/>
       <c r="AA11" s="2">
+        <v>8</v>
+      </c>
+      <c r="AB11" s="2">
         <v>11</v>
       </c>
-      <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
       <c r="AE11" s="3"/>
@@ -2416,30 +2440,40 @@
         <v>8</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3" t="s">
-        <v>87</v>
-      </c>
+      <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
+      <c r="O12" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
+      <c r="Q12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
+      <c r="U12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
@@ -2452,9 +2486,7 @@
       <c r="AF12" s="3"/>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
-      <c r="AI12" s="2">
-        <v>13</v>
-      </c>
+      <c r="AI12" s="3"/>
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
@@ -2469,42 +2501,30 @@
         <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>49</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
-      <c r="U13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="V13" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="U13" s="3"/>
+      <c r="V13" s="3"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
@@ -2518,7 +2538,9 @@
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
-      <c r="AJ13" s="3"/>
+      <c r="AJ13" s="2">
+        <v>13</v>
+      </c>
       <c r="AK13" s="3"/>
       <c r="AL13" s="3"/>
       <c r="AM13" s="3"/>
@@ -2532,14 +2554,12 @@
         <v>10</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>52</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -2551,22 +2571,22 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="V14" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
@@ -2681,21 +2701,21 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AA16" s="3"/>
-      <c r="AB16" s="2">
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="2">
         <v>16</v>
       </c>
-      <c r="AC16" s="2">
+      <c r="AD16" s="2">
         <v>17</v>
       </c>
-      <c r="AD16" s="3"/>
-      <c r="AE16" s="2">
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="2">
         <v>21</v>
       </c>
-      <c r="AF16" s="3"/>
-      <c r="AG16" s="2">
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="2">
         <v>22</v>
       </c>
-      <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
       <c r="AK16" s="3"/>
@@ -2809,14 +2829,12 @@
         <v>15</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -2828,22 +2846,22 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="R19" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="V19" s="3" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
@@ -2874,7 +2892,7 @@
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -2923,7 +2941,7 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -2972,7 +2990,7 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -3021,7 +3039,7 @@
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -3070,7 +3088,7 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -3119,7 +3137,7 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -3131,7 +3149,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -3150,10 +3168,10 @@
       <c r="AA25" s="3"/>
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
-      <c r="AD25" s="2">
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="2">
         <v>28</v>
       </c>
-      <c r="AE25" s="3"/>
       <c r="AF25" s="3"/>
       <c r="AG25" s="3"/>
       <c r="AH25" s="3"/>
@@ -3174,21 +3192,21 @@
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>74</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
@@ -3209,10 +3227,10 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
       <c r="AE26" s="3"/>
-      <c r="AF26" s="2">
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="2">
         <v>30</v>
       </c>
-      <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
       <c r="AI26" s="3"/>
       <c r="AJ26" s="3"/>
@@ -3261,18 +3279,18 @@
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
-      <c r="AC27" s="2">
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="2">
         <v>32</v>
       </c>
-      <c r="AD27" s="3"/>
-      <c r="AE27" s="2">
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="2">
         <v>21</v>
       </c>
-      <c r="AF27" s="3"/>
-      <c r="AG27" s="2">
+      <c r="AG27" s="3"/>
+      <c r="AH27" s="2">
         <v>22</v>
       </c>
-      <c r="AH27" s="3"/>
       <c r="AI27" s="3"/>
       <c r="AJ27" s="3"/>
       <c r="AK27" s="3"/>
@@ -3290,21 +3308,21 @@
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
@@ -3345,21 +3363,21 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
@@ -3457,7 +3475,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
@@ -3484,10 +3502,10 @@
       <c r="AG31" s="3"/>
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
-      <c r="AJ31" s="2">
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="2">
         <v>34</v>
       </c>
-      <c r="AK31" s="3"/>
       <c r="AL31" s="3"/>
       <c r="AM31" s="3"/>
       <c r="AN31" s="3"/>
@@ -3502,7 +3520,7 @@
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
@@ -3512,7 +3530,7 @@
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
@@ -3585,14 +3603,14 @@
       <c r="AB33" s="3"/>
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
-      <c r="AE33" s="2">
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="2">
         <v>36</v>
       </c>
-      <c r="AF33" s="3"/>
-      <c r="AG33" s="2">
+      <c r="AG33" s="3"/>
+      <c r="AH33" s="2">
         <v>22</v>
       </c>
-      <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
       <c r="AJ33" s="3"/>
       <c r="AK33" s="3"/>
@@ -3610,19 +3628,19 @@
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
@@ -3697,10 +3715,10 @@
       <c r="AD35" s="3"/>
       <c r="AE35" s="3"/>
       <c r="AF35" s="3"/>
-      <c r="AG35" s="2">
+      <c r="AG35" s="3"/>
+      <c r="AH35" s="2">
         <v>37</v>
       </c>
-      <c r="AH35" s="3"/>
       <c r="AI35" s="3"/>
       <c r="AJ35" s="3"/>
       <c r="AK35" s="3"/>
@@ -3765,7 +3783,7 @@
         <v>33</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -3782,7 +3800,7 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="P37" s="3"/>
       <c r="Q37" s="3" t="s">
@@ -3794,19 +3812,17 @@
       <c r="S37" s="3"/>
       <c r="T37" s="3"/>
       <c r="U37" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
-      <c r="Y37" s="2">
-        <v>41</v>
-      </c>
+      <c r="Y37" s="3"/>
       <c r="Z37" s="3"/>
-      <c r="AA37" s="2">
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="2">
         <v>42</v>
       </c>
-      <c r="AB37" s="3"/>
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
       <c r="AE37" s="3"/>
@@ -3815,13 +3831,13 @@
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
       <c r="AJ37" s="3"/>
-      <c r="AK37" s="2">
+      <c r="AK37" s="3"/>
+      <c r="AL37" s="2">
         <v>39</v>
       </c>
-      <c r="AL37" s="2">
+      <c r="AM37" s="2">
         <v>40</v>
       </c>
-      <c r="AM37" s="3"/>
       <c r="AN37" s="3"/>
       <c r="AO37" s="3"/>
       <c r="AP37" s="3"/>
@@ -3842,7 +3858,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
@@ -3932,7 +3948,7 @@
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -3944,7 +3960,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
@@ -3963,10 +3979,10 @@
       <c r="AA40" s="3"/>
       <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
-      <c r="AD40" s="2">
+      <c r="AD40" s="3"/>
+      <c r="AE40" s="2">
         <v>46</v>
       </c>
-      <c r="AE40" s="3"/>
       <c r="AF40" s="3"/>
       <c r="AG40" s="3"/>
       <c r="AH40" s="3"/>
@@ -3987,21 +4003,21 @@
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>74</v>
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -4022,10 +4038,10 @@
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
-      <c r="AF41" s="2">
+      <c r="AF41" s="3"/>
+      <c r="AG41" s="2">
         <v>47</v>
       </c>
-      <c r="AG41" s="3"/>
       <c r="AH41" s="3"/>
       <c r="AI41" s="3"/>
       <c r="AJ41" s="3"/>
@@ -4035,9 +4051,7 @@
       <c r="AN41" s="3"/>
       <c r="AO41" s="3"/>
       <c r="AP41" s="3"/>
-      <c r="AQ41" s="2">
-        <v>49</v>
-      </c>
+      <c r="AQ41" s="3"/>
     </row>
     <row r="42" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
@@ -4046,21 +4060,21 @@
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="K42" s="3"/>
       <c r="L42" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
@@ -4118,7 +4132,7 @@
       <c r="S43" s="3"/>
       <c r="T43" s="3"/>
       <c r="U43" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
@@ -4140,17 +4154,17 @@
       <c r="AM43" s="3"/>
       <c r="AN43" s="3"/>
       <c r="AO43" s="3"/>
-      <c r="AP43" s="2">
+      <c r="AP43" s="3"/>
+      <c r="AQ43" s="2">
         <v>48</v>
       </c>
-      <c r="AQ43" s="3"/>
     </row>
     <row r="44" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>40</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -4167,7 +4181,7 @@
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="P44" s="3"/>
       <c r="Q44" s="3" t="s">
@@ -4179,19 +4193,17 @@
       <c r="S44" s="3"/>
       <c r="T44" s="3"/>
       <c r="U44" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
-      <c r="Y44" s="2">
-        <v>41</v>
-      </c>
+      <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
-      <c r="AA44" s="2">
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="2">
         <v>42</v>
       </c>
-      <c r="AB44" s="3"/>
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
       <c r="AE44" s="3"/>
@@ -4200,13 +4212,13 @@
       <c r="AH44" s="3"/>
       <c r="AI44" s="3"/>
       <c r="AJ44" s="3"/>
-      <c r="AK44" s="2">
+      <c r="AK44" s="3"/>
+      <c r="AL44" s="2">
         <v>50</v>
       </c>
-      <c r="AL44" s="2">
+      <c r="AM44" s="2">
         <v>40</v>
       </c>
-      <c r="AM44" s="3"/>
       <c r="AN44" s="3"/>
       <c r="AO44" s="3"/>
       <c r="AP44" s="3"/>
@@ -4216,14 +4228,12 @@
       <c r="A45" s="2">
         <v>41</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="D45" s="3"/>
-      <c r="E45" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -4233,26 +4243,20 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
-      <c r="O45" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="O45" s="3"/>
       <c r="P45" s="3"/>
-      <c r="Q45" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="R45" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
-      <c r="U45" s="3" t="s">
-        <v>84</v>
-      </c>
+      <c r="U45" s="3"/>
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
       <c r="Y45" s="3"/>
-      <c r="Z45" s="3"/>
+      <c r="Z45" s="2">
+        <v>51</v>
+      </c>
       <c r="AA45" s="3"/>
       <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
@@ -4278,7 +4282,7 @@
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
@@ -4334,7 +4338,7 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
@@ -4383,7 +4387,7 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
@@ -4424,7 +4428,7 @@
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -4474,7 +4478,7 @@
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -4484,7 +4488,7 @@
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
@@ -4525,19 +4529,19 @@
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
       <c r="L51" s="3" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -4589,7 +4593,7 @@
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
       <c r="O52" s="3" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
@@ -4662,21 +4666,21 @@
       <c r="Y53" s="3"/>
       <c r="Z53" s="3"/>
       <c r="AA53" s="3"/>
-      <c r="AB53" s="2">
-        <v>56</v>
-      </c>
+      <c r="AB53" s="3"/>
       <c r="AC53" s="2">
+        <v>58</v>
+      </c>
+      <c r="AD53" s="2">
         <v>17</v>
       </c>
-      <c r="AD53" s="3"/>
-      <c r="AE53" s="2">
+      <c r="AE53" s="3"/>
+      <c r="AF53" s="2">
         <v>21</v>
       </c>
-      <c r="AF53" s="3"/>
-      <c r="AG53" s="2">
+      <c r="AG53" s="3"/>
+      <c r="AH53" s="2">
         <v>22</v>
       </c>
-      <c r="AH53" s="3"/>
       <c r="AI53" s="3"/>
       <c r="AJ53" s="3"/>
       <c r="AK53" s="3"/>
@@ -4705,7 +4709,7 @@
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
       <c r="O54" s="3" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="P54" s="3"/>
       <c r="Q54" s="3"/>
@@ -4713,7 +4717,7 @@
       <c r="S54" s="3"/>
       <c r="T54" s="3"/>
       <c r="U54" s="3" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="V54" s="3"/>
       <c r="W54" s="3"/>
@@ -4803,13 +4807,15 @@
       </c>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
+      <c r="D56" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
-      <c r="H56" s="3" t="s">
-        <v>118</v>
-      </c>
+      <c r="H56" s="3"/>
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
@@ -4828,8 +4834,12 @@
       <c r="X56" s="3"/>
       <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
-      <c r="AA56" s="3"/>
-      <c r="AB56" s="3"/>
+      <c r="AA56" s="2">
+        <v>8</v>
+      </c>
+      <c r="AB56" s="2">
+        <v>11</v>
+      </c>
       <c r="AC56" s="3"/>
       <c r="AD56" s="3"/>
       <c r="AE56" s="3"/>
@@ -4840,9 +4850,7 @@
       <c r="AJ56" s="3"/>
       <c r="AK56" s="3"/>
       <c r="AL56" s="3"/>
-      <c r="AM56" s="2">
-        <v>57</v>
-      </c>
+      <c r="AM56" s="3"/>
       <c r="AN56" s="3"/>
       <c r="AO56" s="3"/>
       <c r="AP56" s="3"/>
@@ -4852,28 +4860,38 @@
       <c r="A57" s="2">
         <v>53</v>
       </c>
-      <c r="B57" s="3"/>
+      <c r="B57" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
+      <c r="E57" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
-      <c r="H57" s="3" t="s">
-        <v>118</v>
-      </c>
+      <c r="H57" s="3"/>
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
+      <c r="O57" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
-      <c r="R57" s="3"/>
+      <c r="Q57" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="S57" s="3"/>
       <c r="T57" s="3"/>
-      <c r="U57" s="3"/>
+      <c r="U57" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="V57" s="3"/>
       <c r="W57" s="3"/>
       <c r="X57" s="3"/>
@@ -4891,9 +4909,7 @@
       <c r="AJ57" s="3"/>
       <c r="AK57" s="3"/>
       <c r="AL57" s="3"/>
-      <c r="AM57" s="2">
-        <v>59</v>
-      </c>
+      <c r="AM57" s="3"/>
       <c r="AN57" s="3"/>
       <c r="AO57" s="3"/>
       <c r="AP57" s="3"/>
@@ -4909,19 +4925,17 @@
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
+      <c r="H58" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
-      <c r="L58" s="3" t="s">
-        <v>103</v>
-      </c>
+      <c r="L58" s="3"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
-      <c r="P58" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="P58" s="3"/>
       <c r="Q58" s="3"/>
       <c r="R58" s="3"/>
       <c r="S58" s="3"/>
@@ -4941,13 +4955,13 @@
       <c r="AG58" s="3"/>
       <c r="AH58" s="3"/>
       <c r="AI58" s="3"/>
-      <c r="AJ58" s="2">
-        <v>60</v>
-      </c>
+      <c r="AJ58" s="3"/>
       <c r="AK58" s="3"/>
       <c r="AL58" s="3"/>
       <c r="AM58" s="3"/>
-      <c r="AN58" s="3"/>
+      <c r="AN58" s="2">
+        <v>59</v>
+      </c>
       <c r="AO58" s="3"/>
       <c r="AP58" s="3"/>
       <c r="AQ58" s="3"/>
@@ -4956,17 +4970,15 @@
       <c r="A59" s="2">
         <v>55</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
+      <c r="H59" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
@@ -4980,9 +4992,7 @@
       <c r="S59" s="3"/>
       <c r="T59" s="3"/>
       <c r="U59" s="3"/>
-      <c r="V59" s="3" t="s">
-        <v>76</v>
-      </c>
+      <c r="V59" s="3"/>
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
       <c r="Y59" s="3"/>
@@ -5000,7 +5010,9 @@
       <c r="AK59" s="3"/>
       <c r="AL59" s="3"/>
       <c r="AM59" s="3"/>
-      <c r="AN59" s="3"/>
+      <c r="AN59" s="2">
+        <v>61</v>
+      </c>
       <c r="AO59" s="3"/>
       <c r="AP59" s="3"/>
       <c r="AQ59" s="3"/>
@@ -5011,9 +5023,7 @@
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
-      <c r="D60" s="3" t="s">
-        <v>119</v>
-      </c>
+      <c r="D60" s="3"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -5021,11 +5031,15 @@
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
+      <c r="L60" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
-      <c r="P60" s="3"/>
+      <c r="P60" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="Q60" s="3"/>
       <c r="R60" s="3"/>
       <c r="S60" s="3"/>
@@ -5046,7 +5060,9 @@
       <c r="AH60" s="3"/>
       <c r="AI60" s="3"/>
       <c r="AJ60" s="3"/>
-      <c r="AK60" s="3"/>
+      <c r="AK60" s="2">
+        <v>62</v>
+      </c>
       <c r="AL60" s="3"/>
       <c r="AM60" s="3"/>
       <c r="AN60" s="3"/>
@@ -5058,7 +5074,9 @@
       <c r="A61" s="2">
         <v>57</v>
       </c>
-      <c r="B61" s="3"/>
+      <c r="B61" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -5068,9 +5086,7 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
-      <c r="L61" s="3" t="s">
-        <v>99</v>
-      </c>
+      <c r="L61" s="3"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
@@ -5080,7 +5096,9 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
       <c r="U61" s="3"/>
-      <c r="V61" s="3"/>
+      <c r="V61" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="W61" s="3"/>
       <c r="X61" s="3"/>
       <c r="Y61" s="3"/>
@@ -5109,7 +5127,9 @@
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="D62" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -5117,18 +5137,14 @@
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
-      <c r="L62" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="L62" s="3"/>
       <c r="M62" s="3"/>
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
       <c r="Q62" s="3"/>
       <c r="R62" s="3"/>
-      <c r="S62" s="3" t="s">
-        <v>120</v>
-      </c>
+      <c r="S62" s="3"/>
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
       <c r="V62" s="3"/>
@@ -5149,9 +5165,7 @@
       <c r="AK62" s="3"/>
       <c r="AL62" s="3"/>
       <c r="AM62" s="3"/>
-      <c r="AN62" s="2">
-        <v>63</v>
-      </c>
+      <c r="AN62" s="3"/>
       <c r="AO62" s="3"/>
       <c r="AP62" s="3"/>
       <c r="AQ62" s="3"/>
@@ -5171,7 +5185,7 @@
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
@@ -5220,7 +5234,7 @@
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
@@ -5228,7 +5242,9 @@
       <c r="P64" s="3"/>
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
-      <c r="S64" s="3"/>
+      <c r="S64" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="T64" s="3"/>
       <c r="U64" s="3"/>
       <c r="V64" s="3"/>
@@ -5250,7 +5266,9 @@
       <c r="AL64" s="3"/>
       <c r="AM64" s="3"/>
       <c r="AN64" s="3"/>
-      <c r="AO64" s="3"/>
+      <c r="AO64" s="2">
+        <v>65</v>
+      </c>
       <c r="AP64" s="3"/>
       <c r="AQ64" s="3"/>
     </row>
@@ -5268,12 +5286,12 @@
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
-      <c r="L65" s="3"/>
+      <c r="L65" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
-      <c r="O65" s="3" t="s">
-        <v>107</v>
-      </c>
+      <c r="O65" s="3"/>
       <c r="P65" s="3"/>
       <c r="Q65" s="3"/>
       <c r="R65" s="3"/>
@@ -5317,11 +5335,11 @@
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
-      <c r="L66" s="3"/>
+      <c r="L66" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="M66" s="3"/>
-      <c r="N66" s="3" t="s">
-        <v>102</v>
-      </c>
+      <c r="N66" s="3"/>
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
       <c r="Q66" s="3"/>
@@ -5366,12 +5384,12 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
-      <c r="L67" s="3" t="s">
-        <v>109</v>
-      </c>
+      <c r="L67" s="3"/>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
-      <c r="O67" s="3"/>
+      <c r="O67" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="P67" s="3"/>
       <c r="Q67" s="3"/>
       <c r="R67" s="3"/>
@@ -5411,15 +5429,15 @@
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
-      <c r="H68" s="3" t="s">
-        <v>118</v>
-      </c>
+      <c r="H68" s="3"/>
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
-      <c r="N68" s="3"/>
+      <c r="N68" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
       <c r="Q68" s="3"/>
@@ -5444,9 +5462,7 @@
       <c r="AJ68" s="3"/>
       <c r="AK68" s="3"/>
       <c r="AL68" s="3"/>
-      <c r="AM68" s="2">
-        <v>67</v>
-      </c>
+      <c r="AM68" s="3"/>
       <c r="AN68" s="3"/>
       <c r="AO68" s="3"/>
       <c r="AP68" s="3"/>
@@ -5466,11 +5482,11 @@
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
-      <c r="L69" s="3"/>
+      <c r="L69" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="M69" s="3"/>
-      <c r="N69" s="3" t="s">
-        <v>121</v>
-      </c>
+      <c r="N69" s="3"/>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
       <c r="Q69" s="3"/>
@@ -5505,48 +5521,34 @@
       <c r="A70" s="2">
         <v>66</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>113</v>
-      </c>
+      <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
-      <c r="E70" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
+      <c r="H70" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
-      <c r="O70" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="O70" s="3"/>
       <c r="P70" s="3"/>
-      <c r="Q70" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="R70" s="3" t="s">
-        <v>86</v>
-      </c>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
       <c r="S70" s="3"/>
       <c r="T70" s="3"/>
-      <c r="U70" s="3" t="s">
-        <v>96</v>
-      </c>
+      <c r="U70" s="3"/>
       <c r="V70" s="3"/>
       <c r="W70" s="3"/>
       <c r="X70" s="3"/>
-      <c r="Y70" s="2">
-        <v>41</v>
-      </c>
+      <c r="Y70" s="3"/>
       <c r="Z70" s="3"/>
-      <c r="AA70" s="2">
-        <v>42</v>
-      </c>
+      <c r="AA70" s="3"/>
       <c r="AB70" s="3"/>
       <c r="AC70" s="3"/>
       <c r="AD70" s="3"/>
@@ -5556,14 +5558,12 @@
       <c r="AH70" s="3"/>
       <c r="AI70" s="3"/>
       <c r="AJ70" s="3"/>
-      <c r="AK70" s="2">
+      <c r="AK70" s="3"/>
+      <c r="AL70" s="3"/>
+      <c r="AM70" s="3"/>
+      <c r="AN70" s="2">
         <v>69</v>
       </c>
-      <c r="AL70" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM70" s="3"/>
-      <c r="AN70" s="3"/>
       <c r="AO70" s="3"/>
       <c r="AP70" s="3"/>
       <c r="AQ70" s="3"/>
@@ -5582,11 +5582,11 @@
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
-      <c r="L71" s="3" t="s">
-        <v>104</v>
-      </c>
+      <c r="L71" s="3"/>
       <c r="M71" s="3"/>
-      <c r="N71" s="3"/>
+      <c r="N71" s="3" t="s">
+        <v>124</v>
+      </c>
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
       <c r="Q71" s="3"/>
@@ -5622,7 +5622,7 @@
         <v>68</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -5639,7 +5639,7 @@
       <c r="M72" s="3"/>
       <c r="N72" s="3"/>
       <c r="O72" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="P72" s="3"/>
       <c r="Q72" s="3" t="s">
@@ -5651,19 +5651,17 @@
       <c r="S72" s="3"/>
       <c r="T72" s="3"/>
       <c r="U72" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="V72" s="3"/>
       <c r="W72" s="3"/>
       <c r="X72" s="3"/>
-      <c r="Y72" s="2">
-        <v>41</v>
-      </c>
+      <c r="Y72" s="3"/>
       <c r="Z72" s="3"/>
-      <c r="AA72" s="2">
+      <c r="AA72" s="3"/>
+      <c r="AB72" s="2">
         <v>42</v>
       </c>
-      <c r="AB72" s="3"/>
       <c r="AC72" s="3"/>
       <c r="AD72" s="3"/>
       <c r="AE72" s="3"/>
@@ -5672,13 +5670,13 @@
       <c r="AH72" s="3"/>
       <c r="AI72" s="3"/>
       <c r="AJ72" s="3"/>
-      <c r="AK72" s="2">
-        <v>70</v>
-      </c>
+      <c r="AK72" s="3"/>
       <c r="AL72" s="2">
+        <v>71</v>
+      </c>
+      <c r="AM72" s="2">
         <v>40</v>
       </c>
-      <c r="AM72" s="3"/>
       <c r="AN72" s="3"/>
       <c r="AO72" s="3"/>
       <c r="AP72" s="3"/>
@@ -5698,12 +5696,12 @@
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
-      <c r="L73" s="3"/>
+      <c r="L73" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
-      <c r="O73" s="3" t="s">
-        <v>122</v>
-      </c>
+      <c r="O73" s="3"/>
       <c r="P73" s="3"/>
       <c r="Q73" s="3"/>
       <c r="R73" s="3"/>
@@ -5737,10 +5735,14 @@
       <c r="A74" s="2">
         <v>70</v>
       </c>
-      <c r="B74" s="3"/>
+      <c r="B74" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
+      <c r="E74" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F74" s="3"/>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
@@ -5751,21 +5753,29 @@
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
       <c r="O74" s="3" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="P74" s="3"/>
-      <c r="Q74" s="3"/>
-      <c r="R74" s="3"/>
+      <c r="Q74" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="R74" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="S74" s="3"/>
       <c r="T74" s="3"/>
-      <c r="U74" s="3"/>
+      <c r="U74" s="3" t="s">
+        <v>84</v>
+      </c>
       <c r="V74" s="3"/>
       <c r="W74" s="3"/>
       <c r="X74" s="3"/>
       <c r="Y74" s="3"/>
       <c r="Z74" s="3"/>
       <c r="AA74" s="3"/>
-      <c r="AB74" s="3"/>
+      <c r="AB74" s="2">
+        <v>42</v>
+      </c>
       <c r="AC74" s="3"/>
       <c r="AD74" s="3"/>
       <c r="AE74" s="3"/>
@@ -5775,8 +5785,12 @@
       <c r="AI74" s="3"/>
       <c r="AJ74" s="3"/>
       <c r="AK74" s="3"/>
-      <c r="AL74" s="3"/>
-      <c r="AM74" s="3"/>
+      <c r="AL74" s="2">
+        <v>72</v>
+      </c>
+      <c r="AM74" s="2">
+        <v>40</v>
+      </c>
       <c r="AN74" s="3"/>
       <c r="AO74" s="3"/>
       <c r="AP74" s="3"/>
@@ -5786,14 +5800,10 @@
       <c r="A75" s="2">
         <v>71</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
-      <c r="E75" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
@@ -5804,22 +5814,14 @@
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
       <c r="O75" s="3" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="P75" s="3"/>
-      <c r="Q75" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="R75" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
       <c r="S75" s="3"/>
-      <c r="T75" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="U75" s="3" t="s">
-        <v>111</v>
-      </c>
+      <c r="T75" s="3"/>
+      <c r="U75" s="3"/>
       <c r="V75" s="3"/>
       <c r="W75" s="3"/>
       <c r="X75" s="3"/>
@@ -5839,9 +5841,7 @@
       <c r="AL75" s="3"/>
       <c r="AM75" s="3"/>
       <c r="AN75" s="3"/>
-      <c r="AO75" s="2">
-        <v>73</v>
-      </c>
+      <c r="AO75" s="3"/>
       <c r="AP75" s="3"/>
       <c r="AQ75" s="3"/>
     </row>
@@ -5849,14 +5849,10 @@
       <c r="A76" s="2">
         <v>72</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>110</v>
-      </c>
+      <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
-      <c r="E76" s="3" t="s">
-        <v>110</v>
-      </c>
+      <c r="E76" s="3"/>
       <c r="F76" s="3"/>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
@@ -5867,20 +5863,14 @@
       <c r="M76" s="3"/>
       <c r="N76" s="3"/>
       <c r="O76" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="P76" s="3"/>
-      <c r="Q76" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="R76" s="3" t="s">
-        <v>110</v>
-      </c>
+      <c r="Q76" s="3"/>
+      <c r="R76" s="3"/>
       <c r="S76" s="3"/>
       <c r="T76" s="3"/>
-      <c r="U76" s="3" t="s">
-        <v>110</v>
-      </c>
+      <c r="U76" s="3"/>
       <c r="V76" s="3"/>
       <c r="W76" s="3"/>
       <c r="X76" s="3"/>
@@ -5909,12 +5899,12 @@
         <v>73</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F77" s="3"/>
       <c r="G77" s="3"/>
@@ -5926,19 +5916,21 @@
       <c r="M77" s="3"/>
       <c r="N77" s="3"/>
       <c r="O77" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="P77" s="3"/>
       <c r="Q77" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="R77" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="S77" s="3"/>
-      <c r="T77" s="3"/>
+      <c r="T77" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="U77" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="V77" s="3"/>
       <c r="W77" s="3"/>
@@ -5960,17 +5952,23 @@
       <c r="AM77" s="3"/>
       <c r="AN77" s="3"/>
       <c r="AO77" s="3"/>
-      <c r="AP77" s="3"/>
+      <c r="AP77" s="2">
+        <v>75</v>
+      </c>
       <c r="AQ77" s="3"/>
     </row>
     <row r="78" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>74</v>
       </c>
-      <c r="B78" s="3"/>
+      <c r="B78" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
+      <c r="E78" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="F78" s="3"/>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
@@ -5979,16 +5977,22 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
       <c r="M78" s="3"/>
-      <c r="N78" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="O78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="O78" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="P78" s="3"/>
-      <c r="Q78" s="3"/>
-      <c r="R78" s="3"/>
+      <c r="Q78" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="R78" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="S78" s="3"/>
       <c r="T78" s="3"/>
-      <c r="U78" s="3"/>
+      <c r="U78" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="V78" s="3"/>
       <c r="W78" s="3"/>
       <c r="X78" s="3"/>
@@ -6017,12 +6021,12 @@
         <v>75</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
       <c r="E79" s="3" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="F79" s="3"/>
       <c r="G79" s="3"/>
@@ -6034,30 +6038,26 @@
       <c r="M79" s="3"/>
       <c r="N79" s="3"/>
       <c r="O79" s="3" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="P79" s="3"/>
       <c r="Q79" s="3" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="R79" s="3" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="S79" s="3"/>
       <c r="T79" s="3"/>
       <c r="U79" s="3" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="V79" s="3"/>
       <c r="W79" s="3"/>
       <c r="X79" s="3"/>
-      <c r="Y79" s="2">
-        <v>41</v>
-      </c>
+      <c r="Y79" s="3"/>
       <c r="Z79" s="3"/>
-      <c r="AA79" s="2">
-        <v>42</v>
-      </c>
+      <c r="AA79" s="3"/>
       <c r="AB79" s="3"/>
       <c r="AC79" s="3"/>
       <c r="AD79" s="3"/>
@@ -6067,12 +6067,8 @@
       <c r="AH79" s="3"/>
       <c r="AI79" s="3"/>
       <c r="AJ79" s="3"/>
-      <c r="AK79" s="2">
-        <v>76</v>
-      </c>
-      <c r="AL79" s="2">
-        <v>40</v>
-      </c>
+      <c r="AK79" s="3"/>
+      <c r="AL79" s="3"/>
       <c r="AM79" s="3"/>
       <c r="AN79" s="3"/>
       <c r="AO79" s="3"/>
@@ -6095,10 +6091,10 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
       <c r="M80" s="3"/>
-      <c r="N80" s="3"/>
-      <c r="O80" s="3" t="s">
-        <v>124</v>
-      </c>
+      <c r="N80" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="O80" s="3"/>
       <c r="P80" s="3"/>
       <c r="Q80" s="3"/>
       <c r="R80" s="3"/>
@@ -6128,17 +6124,17 @@
       <c r="AP80" s="3"/>
       <c r="AQ80" s="3"/>
     </row>
-    <row r="81" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:43" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>77</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="3"/>
       <c r="E81" s="3" t="s">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
@@ -6150,19 +6146,19 @@
       <c r="M81" s="3"/>
       <c r="N81" s="3"/>
       <c r="O81" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="P81" s="3"/>
       <c r="Q81" s="3" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="R81" s="3" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
       <c r="U81" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="V81" s="3"/>
       <c r="W81" s="3"/>
@@ -6170,7 +6166,9 @@
       <c r="Y81" s="3"/>
       <c r="Z81" s="3"/>
       <c r="AA81" s="3"/>
-      <c r="AB81" s="3"/>
+      <c r="AB81" s="2">
+        <v>42</v>
+      </c>
       <c r="AC81" s="3"/>
       <c r="AD81" s="3"/>
       <c r="AE81" s="3"/>
@@ -6180,18 +6178,131 @@
       <c r="AI81" s="3"/>
       <c r="AJ81" s="3"/>
       <c r="AK81" s="3"/>
-      <c r="AL81" s="3"/>
-      <c r="AM81" s="3"/>
+      <c r="AL81" s="2">
+        <v>78</v>
+      </c>
+      <c r="AM81" s="2">
+        <v>40</v>
+      </c>
       <c r="AN81" s="3"/>
       <c r="AO81" s="3"/>
       <c r="AP81" s="3"/>
+      <c r="AQ81" s="3"/>
+    </row>
+    <row r="82" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A82" s="2">
+        <v>78</v>
+      </c>
+      <c r="B82" s="3"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="P82" s="3"/>
+      <c r="Q82" s="3"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="3"/>
+      <c r="T82" s="3"/>
+      <c r="U82" s="3"/>
+      <c r="V82" s="3"/>
+      <c r="W82" s="3"/>
+      <c r="X82" s="3"/>
+      <c r="Y82" s="3"/>
+      <c r="Z82" s="3"/>
+      <c r="AA82" s="3"/>
+      <c r="AB82" s="3"/>
+      <c r="AC82" s="3"/>
+      <c r="AD82" s="3"/>
+      <c r="AE82" s="3"/>
+      <c r="AF82" s="3"/>
+      <c r="AG82" s="3"/>
+      <c r="AH82" s="3"/>
+      <c r="AI82" s="3"/>
+      <c r="AJ82" s="3"/>
+      <c r="AK82" s="3"/>
+      <c r="AL82" s="3"/>
+      <c r="AM82" s="3"/>
+      <c r="AN82" s="3"/>
+      <c r="AO82" s="3"/>
+      <c r="AP82" s="3"/>
+      <c r="AQ82" s="3"/>
+    </row>
+    <row r="83" spans="1:43" x14ac:dyDescent="0.35">
+      <c r="A83" s="2">
+        <v>79</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+      <c r="E83" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="3"/>
+      <c r="J83" s="3"/>
+      <c r="K83" s="3"/>
+      <c r="L83" s="3"/>
+      <c r="M83" s="3"/>
+      <c r="N83" s="3"/>
+      <c r="O83" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="P83" s="3"/>
+      <c r="Q83" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="R83" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="S83" s="3"/>
+      <c r="T83" s="3"/>
+      <c r="U83" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="V83" s="3"/>
+      <c r="W83" s="3"/>
+      <c r="X83" s="3"/>
+      <c r="Y83" s="3"/>
+      <c r="Z83" s="3"/>
+      <c r="AA83" s="3"/>
+      <c r="AB83" s="3"/>
+      <c r="AC83" s="3"/>
+      <c r="AD83" s="3"/>
+      <c r="AE83" s="3"/>
+      <c r="AF83" s="3"/>
+      <c r="AG83" s="3"/>
+      <c r="AH83" s="3"/>
+      <c r="AI83" s="3"/>
+      <c r="AJ83" s="3"/>
+      <c r="AK83" s="3"/>
+      <c r="AL83" s="3"/>
+      <c r="AM83" s="3"/>
+      <c r="AN83" s="3"/>
+      <c r="AO83" s="3"/>
+      <c r="AP83" s="3"/>
+      <c r="AQ83" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A1:AP1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:V2"/>
-    <mergeCell ref="W2:AP2"/>
+    <mergeCell ref="A1:AQ1"/>
+    <mergeCell ref="W2:AQ2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>